<commit_message>
Add files P1 Session 2
</commit_message>
<xml_diff>
--- a/2020-cubic.xlsx
+++ b/2020-cubic.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayte\Desktop\ED_WorkSpace\ED-2020-21-FernandezCoroMariaTeresa-UO263728\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4545759A-B6C3-4B3B-91F5-AE14319BA248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{094E2459-FF40-4411-AD2F-FEF4629C8B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="2020-cubic" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Valor n</t>
+    <t>Milisegundos</t>
   </si>
   <si>
-    <t>Milisegundos</t>
+    <t>Valor n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,19 +548,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -687,10 +684,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -701,16 +695,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -830,94 +819,94 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>109</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>211</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>377</c:v>
+                  <c:v>383</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>593</c:v>
+                  <c:v>652</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>899</c:v>
+                  <c:v>911</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1270</c:v>
+                  <c:v>1452</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1777</c:v>
+                  <c:v>1962</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2332</c:v>
+                  <c:v>2396</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3033</c:v>
+                  <c:v>3205</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3822</c:v>
+                  <c:v>4032</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4781</c:v>
+                  <c:v>5061</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6044</c:v>
+                  <c:v>6066</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7566</c:v>
+                  <c:v>7387</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8612</c:v>
+                  <c:v>8699</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10156</c:v>
+                  <c:v>10293</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11937</c:v>
+                  <c:v>11822</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13948</c:v>
+                  <c:v>14146</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>16109</c:v>
+                  <c:v>16423</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18559</c:v>
+                  <c:v>18619</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21163</c:v>
+                  <c:v>21392</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24104</c:v>
+                  <c:v>24139</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>27285</c:v>
+                  <c:v>27806</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>30656</c:v>
+                  <c:v>31483</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34339</c:v>
+                  <c:v>34602</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>38263</c:v>
+                  <c:v>38644</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42566</c:v>
+                  <c:v>42630</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>47038</c:v>
+                  <c:v>47588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -925,7 +914,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5430-4B3B-A789-16A688CE688C}"/>
+              <c16:uniqueId val="{00000000-FE47-42D8-BCEA-C8C85B56C861}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -939,11 +928,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="421991160"/>
-        <c:axId val="421988208"/>
+        <c:axId val="426346824"/>
+        <c:axId val="426345840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421991160"/>
+        <c:axId val="426346824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -986,7 +975,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421988208"/>
+        <c:crossAx val="426345840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -994,7 +983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421988208"/>
+        <c:axId val="426345840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1034,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421991160"/>
+        <c:crossAx val="426346824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1648,23 +1637,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D2395CB-21B2-43DC-8821-D95A1DD23BC0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95EB33B3-F453-4877-A95C-192909C1EF68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1981,273 +1970,272 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
+      <c r="B3" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>47</v>
+      <c r="B5" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>109</v>
+      <c r="B6" s="1">
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <v>211</v>
+      <c r="B7" s="1">
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <v>377</v>
+      <c r="B8" s="1">
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <v>593</v>
+      <c r="B9" s="1">
+        <v>652</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>899</v>
+      <c r="B10" s="1">
+        <v>911</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <v>1270</v>
+      <c r="B11" s="1">
+        <v>1452</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <v>1777</v>
+      <c r="B12" s="1">
+        <v>1962</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <v>2332</v>
+      <c r="B13" s="1">
+        <v>2396</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <v>3033</v>
+      <c r="B14" s="1">
+        <v>3205</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
-        <v>3822</v>
+      <c r="B15" s="1">
+        <v>4032</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
-        <v>4781</v>
+      <c r="B16" s="1">
+        <v>5061</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <v>6044</v>
+      <c r="B17" s="1">
+        <v>6066</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
-        <v>7566</v>
+      <c r="B18" s="1">
+        <v>7387</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
-        <v>8612</v>
+      <c r="B19" s="1">
+        <v>8699</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="3">
-        <v>10156</v>
+      <c r="B20" s="1">
+        <v>10293</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="3">
-        <v>11937</v>
+      <c r="B21" s="1">
+        <v>11822</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
-        <v>13948</v>
+      <c r="B22" s="1">
+        <v>14146</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
-        <v>16109</v>
+      <c r="B23" s="1">
+        <v>16423</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
-        <v>18559</v>
+      <c r="B24" s="1">
+        <v>18619</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
-        <v>21163</v>
+      <c r="B25" s="1">
+        <v>21392</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="3">
-        <v>24104</v>
+      <c r="B26" s="1">
+        <v>24139</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="3">
-        <v>27285</v>
+      <c r="B27" s="1">
+        <v>27806</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="3">
-        <v>30656</v>
+      <c r="B28" s="1">
+        <v>31483</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="3">
-        <v>34339</v>
+      <c r="B29" s="1">
+        <v>34602</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
-        <v>38263</v>
+      <c r="B30" s="1">
+        <v>38644</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="3">
-        <v>42566</v>
+      <c r="B31" s="1">
+        <v>42630</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="4">
-        <v>47038</v>
+      <c r="B32" s="2">
+        <v>47588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>